<commit_message>
Adapting to new gfx-three-js usage.
</commit_message>
<xml_diff>
--- a/doc/ChanSlope.xlsx
+++ b/doc/ChanSlope.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="640" windowWidth="25600" windowHeight="12240" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="50460" windowHeight="28340" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -942,7 +942,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -952,7 +952,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1">
-        <v>-0.8</v>
+        <v>-0.05</v>
       </c>
       <c r="C1">
         <v>4</v>
@@ -981,23 +981,23 @@
       </c>
       <c r="C3" s="1">
         <f>1/(POWER(C1*C1/B3,A1))</f>
-        <v>9.189586839976279</v>
+        <v>1.1486983549970351</v>
       </c>
       <c r="D3" s="1">
         <f>1/(POWER(D1*D1/B3,A1))</f>
-        <v>84.4485062894652</v>
+        <v>1.3195079107728942</v>
       </c>
       <c r="E3" s="1">
         <f>1/(POWER(E1*E1/B3,A1))</f>
-        <v>776.04688205332377</v>
+        <v>1.515716566510398</v>
       </c>
       <c r="F3" s="1">
         <f>1/(POWER(F1*F1/B3,A1))</f>
-        <v>2352.5342310339279</v>
+        <v>1.6245047927124709</v>
       </c>
       <c r="G3" s="1">
         <f>1/(POWER(G1*G1/B3,A1))</f>
-        <v>7131.5502145218443</v>
+        <v>1.7411011265922482</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1006,23 +1006,23 @@
       </c>
       <c r="C4" s="1">
         <f>1/(POWER(C1*C1/B4,A1))</f>
-        <v>3.031433133020796</v>
+        <v>1.0717734625362931</v>
       </c>
       <c r="D4" s="1">
         <f>1/(POWER(D1*D1/B4,A1))</f>
-        <v>27.857618025475972</v>
+        <v>1.2311444133449163</v>
       </c>
       <c r="E4" s="1">
         <f>1/(POWER(E1*E1/B4,A1))</f>
-        <v>256.00000000000017</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="F4" s="1">
         <f>1/(POWER(F1*F1/B4,A1))</f>
-        <v>776.04688205332377</v>
+        <v>1.515716566510398</v>
       </c>
       <c r="G4" s="1">
         <f>1/(POWER(G1*G1/B4,A1))</f>
-        <v>2352.5342310339279</v>
+        <v>1.6245047927124709</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1035,19 +1035,19 @@
       </c>
       <c r="D5" s="1">
         <f>1/(POWER(D1*D1/B5,A1))</f>
-        <v>9.189586839976279</v>
+        <v>1.1486983549970351</v>
       </c>
       <c r="E5" s="1">
         <f>1/(POWER(E1*E1/B5,A1))</f>
-        <v>84.4485062894652</v>
+        <v>1.3195079107728942</v>
       </c>
       <c r="F5" s="1">
         <f>1/(POWER(F1*F1/B5,A1))</f>
-        <v>256.00000000000017</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="G5" s="1">
         <f>1/(POWER(G1*G1/B5,A1))</f>
-        <v>776.04688205332377</v>
+        <v>1.515716566510398</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1057,19 +1057,19 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1">
         <f>1/(POWER(D1*D1/B6,A1))</f>
-        <v>3.031433133020796</v>
+        <v>1.0717734625362931</v>
       </c>
       <c r="E6" s="1">
         <f>1/(POWER(E1*E1/B6,A1))</f>
-        <v>27.857618025475972</v>
+        <v>1.2311444133449163</v>
       </c>
       <c r="F6" s="1">
         <f>1/(POWER(F1*F1/B6,A1))</f>
-        <v>84.4485062894652</v>
+        <v>1.3195079107728942</v>
       </c>
       <c r="G6" s="1">
         <f>1/(POWER(G1*G1/B6,A1))</f>
-        <v>256.00000000000017</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1079,19 +1079,19 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1">
         <f>1/(POWER(D1*D1/B7,A1))</f>
-        <v>1.7411011265922482</v>
+        <v>1.0352649238413776</v>
       </c>
       <c r="E7" s="1">
         <f>1/(POWER(E1*E1/B7,A1))</f>
-        <v>16.000000000000007</v>
+        <v>1.189207115002721</v>
       </c>
       <c r="F7" s="1">
         <f>1/(POWER(F1*F1/B7,A1))</f>
-        <v>48.502930128332743</v>
+        <v>1.2745606273192622</v>
       </c>
       <c r="G7" s="1">
         <f>1/(POWER(G1*G1/B7,A1))</f>
-        <v>147.03338943962058</v>
+        <v>1.3660402567543957</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1105,15 +1105,15 @@
       </c>
       <c r="E8" s="1">
         <f>1/(POWER(E1*E1/B8,A1))</f>
-        <v>9.189586839976279</v>
+        <v>1.1486983549970351</v>
       </c>
       <c r="F8" s="1">
         <f>1/(POWER(F1*F1/B8,A1))</f>
-        <v>27.857618025475972</v>
+        <v>1.2311444133449163</v>
       </c>
       <c r="G8" s="1">
         <f>1/(POWER(G1*G1/B8,A1))</f>
-        <v>84.4485062894652</v>
+        <v>1.3195079107728942</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1126,11 +1126,11 @@
       </c>
       <c r="F9" s="1">
         <f>1/(POWER(F1*F1/B9,A1))</f>
-        <v>3.031433133020796</v>
+        <v>1.0717734625362931</v>
       </c>
       <c r="G9" s="1">
         <f>1/(POWER(G1*G1/B9,A1))</f>
-        <v>9.189586839976279</v>
+        <v>1.1486983549970351</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="G10" s="1">
         <f>1/(POWER(G1*G1/B10,A1))</f>
-        <v>3.031433133020796</v>
+        <v>1.0717734625362931</v>
       </c>
     </row>
     <row r="11" spans="1:7">

</xml_diff>